<commit_message>
changed lots of cards
</commit_message>
<xml_diff>
--- a/footballers.xlsx
+++ b/footballers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfc90\Desktop\Footballteam\footballteam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I852780\Desktop\football team\footballteam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1B93589-E958-42F1-876E-DBF9FC577F05}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8370D087-6293-4C73-BC43-3FDF31CEAE3B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11250" windowHeight="7560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,15 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Footballers</t>
   </si>
@@ -53,9 +52,6 @@
     <t>Can re-roll 1 die</t>
   </si>
   <si>
-    <t>When you succeed in an assist test, if there is another test on the same event cards, you can roll 1 more die</t>
-  </si>
-  <si>
     <t>Footballer 1</t>
   </si>
   <si>
@@ -92,9 +88,6 @@
     <t>Footballer 12</t>
   </si>
   <si>
-    <t>When you succeed in a shooting test, gain 3 gold</t>
-  </si>
-  <si>
     <t>Star counts as 2</t>
   </si>
   <si>
@@ -111,6 +104,39 @@
   </si>
   <si>
     <t>Roll for defence as if was rolling for a shooting test</t>
+  </si>
+  <si>
+    <t>When you succeed in an assist test, roll +1 die for other tests in the card</t>
+  </si>
+  <si>
+    <t>Highest</t>
+  </si>
+  <si>
+    <t>Footballer 16</t>
+  </si>
+  <si>
+    <t>When you succeed in a shooting test, gain 1 gold</t>
+  </si>
+  <si>
+    <t>When you succeed in a defence test, draw 1 card</t>
+  </si>
+  <si>
+    <t>Footballer 17</t>
+  </si>
+  <si>
+    <t>Ignore all tests with a difficulty of 2 or less</t>
+  </si>
+  <si>
+    <t>Footballer 18</t>
+  </si>
+  <si>
+    <t>Footballer 19</t>
+  </si>
+  <si>
+    <t>When you pass a test, banish a card from the table</t>
+  </si>
+  <si>
+    <t>Stars count as 2</t>
   </si>
 </sst>
 </file>
@@ -179,7 +205,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -478,10 +504,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -491,15 +517,15 @@
     <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="7" width="96.140625" customWidth="1"/>
-    <col min="11" max="11" width="29.42578125" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" customWidth="1"/>
-    <col min="14" max="14" width="37" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" customWidth="1"/>
+    <col min="6" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="96.140625" customWidth="1"/>
+    <col min="12" max="12" width="29.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" customWidth="1"/>
+    <col min="15" max="15" width="37" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -519,241 +545,286 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2">
+        <f>SUM(C2:E2)</f>
+        <v>4</v>
+      </c>
+      <c r="G2" s="2">
+        <f>MAX(C2:E2)</f>
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2">
-        <f t="shared" ref="F2:F16" si="0">SUM(C2:E2)</f>
-        <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <f>SUM(C3:E3)</f>
+        <v>4</v>
+      </c>
+      <c r="G3" s="2">
+        <f>MAX(C3:E3)</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <f>SUM(C4:E4)</f>
+        <v>4</v>
+      </c>
+      <c r="G4" s="2">
+        <f>MAX(C4:E4)</f>
+        <v>2</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <f>SUM(C5:E5)</f>
+        <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <f>MAX(C5:E5)</f>
+        <v>2</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>2</v>
-      </c>
-      <c r="F3" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2">
+        <f>SUM(C6:E6)</f>
+        <v>5</v>
+      </c>
+      <c r="G6" s="2">
+        <f>MAX(C6:E6)</f>
+        <v>3</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>3</v>
-      </c>
-      <c r="F4" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2">
+        <f>SUM(C7:E7)</f>
+        <v>6</v>
+      </c>
+      <c r="G7" s="2">
+        <f>MAX(C7:E7)</f>
+        <v>3</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2">
+        <f>SUM(C8:E8)</f>
+        <v>5</v>
+      </c>
+      <c r="G8" s="2">
+        <f>MAX(C8:E8)</f>
+        <v>2</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
-      </c>
-      <c r="F5" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2">
-        <v>2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>3</v>
-      </c>
-      <c r="F7" s="2">
-        <f t="shared" si="0"/>
+      <c r="B9" s="2">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2">
+        <f>SUM(C9:E9)</f>
         <v>6</v>
       </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="G9" s="2">
+        <f>MAX(C9:E9)</f>
+        <v>3</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="F10" s="2">
+        <f>SUM(C10:E10)</f>
+        <v>6</v>
+      </c>
+      <c r="G10" s="2">
+        <f>MAX(C10:E10)</f>
+        <v>3</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <f>SUM(C11:E11)</f>
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <f>MAX(C11:E11)</f>
+        <v>3</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" s="2">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2">
-        <v>3</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2">
-        <v>2</v>
-      </c>
-      <c r="E10" s="2">
-        <v>2</v>
-      </c>
-      <c r="F10" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="2">
-        <v>7</v>
-      </c>
-      <c r="C11" s="2">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2">
-        <v>2</v>
-      </c>
-      <c r="E11" s="2">
-        <v>3</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="B12" s="2">
         <v>6</v>
@@ -765,19 +836,23 @@
         <v>2</v>
       </c>
       <c r="E12" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <f>SUM(C12:E12)</f>
+        <v>6</v>
+      </c>
+      <c r="G12" s="2">
+        <f>MAX(C12:E12)</f>
+        <v>2</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2">
         <v>8</v>
@@ -786,98 +861,224 @@
         <v>2</v>
       </c>
       <c r="D13" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E13" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(C13:E13)</f>
+        <v>7</v>
+      </c>
+      <c r="G13" s="2">
+        <f>MAX(C13:E13)</f>
+        <v>3</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2">
         <v>8</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="C14" s="2">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2">
+        <f>SUM(C14:E14)</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="2">
-        <v>4</v>
-      </c>
-      <c r="C14" s="2">
-        <v>3</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="2">
+        <f>MAX(C14:E14)</f>
+        <v>3</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2">
+        <f>SUM(C15:E15)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="G15" s="2">
+        <f>MAX(C15:E15)</f>
+        <v>4</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="2">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2">
+        <f>SUM(C16:E16)</f>
+        <v>8</v>
+      </c>
+      <c r="G16" s="2">
+        <f>MAX(C16:E16)</f>
+        <v>4</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+      <c r="F17" s="2">
+        <f>SUM(C17:E17)</f>
+        <v>7</v>
+      </c>
+      <c r="G17" s="2">
+        <f>MAX(C17:E17)</f>
+        <v>4</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="2">
-        <v>6</v>
-      </c>
-      <c r="C15" s="2">
-        <v>3</v>
-      </c>
-      <c r="D15" s="2">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="2">
-        <v>8</v>
-      </c>
-      <c r="C16" s="2">
-        <v>3</v>
-      </c>
-      <c r="D16" s="2">
-        <v>3</v>
-      </c>
-      <c r="E16" s="2">
-        <v>3</v>
-      </c>
-      <c r="F16" s="2">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="25" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="12.75" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="2">
+        <v>11</v>
+      </c>
+      <c r="C18" s="2">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2">
+        <f>SUM(C18:E18)</f>
+        <v>10</v>
+      </c>
+      <c r="G18" s="2">
+        <f>MAX(C18:E18)</f>
+        <v>5</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="2">
+        <v>12</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2">
+        <f>SUM(C19:E19)</f>
+        <v>10</v>
+      </c>
+      <c r="G19" s="2">
+        <f>MAX(C19:E19)</f>
+        <v>5</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="2">
+        <v>14</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3</v>
+      </c>
+      <c r="D20" s="2">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2">
+        <v>4</v>
+      </c>
+      <c r="F20" s="2">
+        <f>SUM(C20:E20)</f>
+        <v>12</v>
+      </c>
+      <c r="G20" s="2">
+        <f>MAX(C20:E20)</f>
+        <v>5</v>
+      </c>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{9B31C678-E6F5-4218-9CE9-513CAEF67B0C}">
-    <sortState ref="A2:H16">
-      <sortCondition ref="C1"/>
+  <autoFilter ref="A1:I1" xr:uid="{9B31C678-E6F5-4218-9CE9-513CAEF67B0C}">
+    <sortState ref="A2:I20">
+      <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>